<commit_message>
Fill in more depth change values
</commit_message>
<xml_diff>
--- a/data/poloczanska2013NCC/nceas.999.1_depth.xlsx
+++ b/data/poloczanska2013NCC/nceas.999.1_depth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpinsky/Documents/Rutgers/ARMS review/data/poloczanska2013NCC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpinsky/Documents/Rutgers/ARMS review/ARMS_ClimateShift/data/poloczanska2013NCC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA84C741-C7AE-CB42-A7BD-9C846CD7695B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA289901-764F-9040-9816-A1E4EBF43DC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{0655E902-D71A-964F-A7E6-2698D6831411}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5759" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5800" uniqueCount="334">
   <si>
     <t>unique</t>
   </si>
@@ -8639,7 +8639,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F60B313-2417-5B4F-9ED9-A101CFCB5EEE}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1F60B313-2417-5B4F-9ED9-A101CFCB5EEE}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="67">
     <pivotField showAll="0"/>
@@ -9058,22 +9058,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC71C5B-AB58-0B49-91AB-FB9C010227A8}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:BP107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AS31" sqref="AS31"/>
+      <selection pane="bottomLeft" activeCell="BP31" sqref="BP31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="5" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="23" width="0" hidden="1" customWidth="1"/>
-    <col min="26" max="39" width="0" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="23" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="26" max="27" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="10.83203125" customWidth="1"/>
+    <col min="29" max="33" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="10.83203125" customWidth="1"/>
+    <col min="35" max="37" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="38" max="39" width="10.83203125" customWidth="1"/>
+    <col min="41" max="41" width="10.83203125" customWidth="1"/>
     <col min="52" max="67" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22674,6 +22678,9 @@
       <c r="BO67" t="s">
         <v>272</v>
       </c>
+      <c r="BP67" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A68">
@@ -22874,8 +22881,11 @@
       <c r="BO68" t="s">
         <v>272</v>
       </c>
+      <c r="BP68" t="s">
+        <v>333</v>
+      </c>
     </row>
-    <row r="69" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1251</v>
       </c>
@@ -23074,8 +23084,11 @@
       <c r="BO69" t="s">
         <v>278</v>
       </c>
+      <c r="BP69" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="70" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1252</v>
       </c>
@@ -23274,8 +23287,11 @@
       <c r="BO70" t="s">
         <v>278</v>
       </c>
+      <c r="BP70" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="71" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1253</v>
       </c>
@@ -23474,8 +23490,11 @@
       <c r="BO71" t="s">
         <v>278</v>
       </c>
+      <c r="BP71" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="72" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1254</v>
       </c>
@@ -23674,8 +23693,11 @@
       <c r="BO72" t="s">
         <v>278</v>
       </c>
+      <c r="BP72" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="73" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1255</v>
       </c>
@@ -23874,8 +23896,11 @@
       <c r="BO73" t="s">
         <v>278</v>
       </c>
+      <c r="BP73" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="74" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1256</v>
       </c>
@@ -24074,8 +24099,11 @@
       <c r="BO74" t="s">
         <v>278</v>
       </c>
+      <c r="BP74" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="75" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1257</v>
       </c>
@@ -24274,8 +24302,11 @@
       <c r="BO75" t="s">
         <v>278</v>
       </c>
+      <c r="BP75" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="76" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1258</v>
       </c>
@@ -24474,8 +24505,11 @@
       <c r="BO76" t="s">
         <v>278</v>
       </c>
+      <c r="BP76" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="77" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1259</v>
       </c>
@@ -24674,8 +24708,11 @@
       <c r="BO77" t="s">
         <v>278</v>
       </c>
+      <c r="BP77" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="78" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1260</v>
       </c>
@@ -24874,8 +24911,11 @@
       <c r="BO78" t="s">
         <v>278</v>
       </c>
+      <c r="BP78" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="79" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1261</v>
       </c>
@@ -25074,8 +25114,11 @@
       <c r="BO79" t="s">
         <v>278</v>
       </c>
+      <c r="BP79" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="80" spans="1:68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1262</v>
       </c>
@@ -25274,8 +25317,11 @@
       <c r="BO80" t="s">
         <v>278</v>
       </c>
+      <c r="BP80" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="81" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1263</v>
       </c>
@@ -25474,8 +25520,11 @@
       <c r="BO81" t="s">
         <v>278</v>
       </c>
+      <c r="BP81" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="82" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1264</v>
       </c>
@@ -25674,8 +25723,11 @@
       <c r="BO82" t="s">
         <v>278</v>
       </c>
+      <c r="BP82" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="83" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1265</v>
       </c>
@@ -25874,8 +25926,11 @@
       <c r="BO83" t="s">
         <v>278</v>
       </c>
+      <c r="BP83" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="84" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1266</v>
       </c>
@@ -26074,8 +26129,11 @@
       <c r="BO84" t="s">
         <v>278</v>
       </c>
+      <c r="BP84" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="85" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1294</v>
       </c>
@@ -26274,8 +26332,11 @@
       <c r="BO85" t="s">
         <v>278</v>
       </c>
+      <c r="BP85" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="86" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1295</v>
       </c>
@@ -26474,8 +26535,11 @@
       <c r="BO86" t="s">
         <v>278</v>
       </c>
+      <c r="BP86" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="87" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1296</v>
       </c>
@@ -26674,8 +26738,11 @@
       <c r="BO87" t="s">
         <v>278</v>
       </c>
+      <c r="BP87" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="88" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1297</v>
       </c>
@@ -26874,8 +26941,11 @@
       <c r="BO88" t="s">
         <v>278</v>
       </c>
+      <c r="BP88" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="89" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1298</v>
       </c>
@@ -27074,8 +27144,11 @@
       <c r="BO89" t="s">
         <v>278</v>
       </c>
+      <c r="BP89" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="90" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1299</v>
       </c>
@@ -27274,8 +27347,11 @@
       <c r="BO90" t="s">
         <v>278</v>
       </c>
+      <c r="BP90" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="91" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1300</v>
       </c>
@@ -27474,8 +27550,11 @@
       <c r="BO91" t="s">
         <v>278</v>
       </c>
+      <c r="BP91" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="92" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1301</v>
       </c>
@@ -27674,8 +27753,11 @@
       <c r="BO92" t="s">
         <v>278</v>
       </c>
+      <c r="BP92" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="93" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1302</v>
       </c>
@@ -27874,8 +27956,11 @@
       <c r="BO93" t="s">
         <v>278</v>
       </c>
+      <c r="BP93" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="94" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1303</v>
       </c>
@@ -28074,8 +28159,11 @@
       <c r="BO94" t="s">
         <v>278</v>
       </c>
+      <c r="BP94" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="95" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1304</v>
       </c>
@@ -28274,8 +28362,11 @@
       <c r="BO95" t="s">
         <v>278</v>
       </c>
+      <c r="BP95" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="96" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1305</v>
       </c>
@@ -28474,8 +28565,11 @@
       <c r="BO96" t="s">
         <v>278</v>
       </c>
+      <c r="BP96" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="97" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1306</v>
       </c>
@@ -28674,8 +28768,11 @@
       <c r="BO97" t="s">
         <v>278</v>
       </c>
+      <c r="BP97" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="98" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1307</v>
       </c>
@@ -28874,8 +28971,11 @@
       <c r="BO98" t="s">
         <v>278</v>
       </c>
+      <c r="BP98" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="99" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1308</v>
       </c>
@@ -29074,8 +29174,11 @@
       <c r="BO99" t="s">
         <v>278</v>
       </c>
+      <c r="BP99" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="100" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1309</v>
       </c>
@@ -29274,8 +29377,11 @@
       <c r="BO100" t="s">
         <v>278</v>
       </c>
+      <c r="BP100" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="101" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1310</v>
       </c>
@@ -29474,8 +29580,11 @@
       <c r="BO101" t="s">
         <v>278</v>
       </c>
+      <c r="BP101" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="102" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1311</v>
       </c>
@@ -29674,8 +29783,11 @@
       <c r="BO102" t="s">
         <v>278</v>
       </c>
+      <c r="BP102" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="103" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1312</v>
       </c>
@@ -29874,8 +29986,11 @@
       <c r="BO103" t="s">
         <v>278</v>
       </c>
+      <c r="BP103" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="104" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1317</v>
       </c>
@@ -30074,8 +30189,11 @@
       <c r="BO104" t="s">
         <v>278</v>
       </c>
+      <c r="BP104" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="105" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2381</v>
       </c>
@@ -30274,8 +30392,11 @@
       <c r="BO105" t="s">
         <v>278</v>
       </c>
+      <c r="BP105" t="s">
+        <v>333</v>
+      </c>
     </row>
-    <row r="106" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2382</v>
       </c>
@@ -30474,8 +30595,11 @@
       <c r="BO106" t="s">
         <v>278</v>
       </c>
+      <c r="BP106" t="s">
+        <v>333</v>
+      </c>
     </row>
-    <row r="107" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2383</v>
       </c>
@@ -30674,17 +30798,12 @@
       <c r="BO107" t="s">
         <v>278</v>
       </c>
+      <c r="BP107" t="s">
+        <v>333</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BO107" xr:uid="{7694D620-BDEB-6248-821F-04039E083C8A}">
-    <filterColumn colId="39">
-      <filters>
-        <filter val="Negative"/>
-        <filter val="No change"/>
-        <filter val="Positive"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:BO107" xr:uid="{7694D620-BDEB-6248-821F-04039E083C8A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>